<commit_message>
Added dec 21 classes
</commit_message>
<xml_diff>
--- a/bin/testData/Book1.xlsx
+++ b/bin/testData/Book1.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chbha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Java\new\selenium-automation\src\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0E68F6-2399-4B40-A32B-A6BEA9ED2D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFCDD66-E038-4E1A-865F-63CB140532A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{32AB1F36-F464-4CB0-9CFE-11E3E0644329}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{32AB1F36-F464-4CB0-9CFE-11E3E0644329}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="signup" sheetId="2" r:id="rId2"/>
+    <sheet name="myInfo" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>email</t>
   </si>
@@ -41,13 +43,70 @@
   </si>
   <si>
     <t>abcd</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>emailid</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>peter</t>
+  </si>
+  <si>
+    <t>some@gmail</t>
+  </si>
+  <si>
+    <t>david</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s@gmail</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>DrivingLicenceNumber</t>
+  </si>
+  <si>
+    <t>EID</t>
+  </si>
+  <si>
+    <t>MaritalStatus</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Un married</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,13 +114,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,13 +152,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EDB671-A85B-40EA-ACBE-7613B9E7FC6C}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,10 +489,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -419,9 +504,209 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F20">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F51071-F08C-4F60-92EE-E04232792D92}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44614</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44249</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44249</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>44249</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44249</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44249</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5E61C403-534D-40D1-BD92-8ECE5B7C140B}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{3E5BA596-2589-4735-A8DD-DC9E5E9CAFF8}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{4FD735BF-7B4B-4813-B787-14D84B54ED61}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{09E04B61-482F-41AD-8FB4-0030A76C6A20}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{98F83E3E-FF46-4891-A146-42A7C7C6E3A5}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{6D68A9EB-C81E-412E-AA75-F0DBE360D83B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1D2C35-A9F4-4D0A-9452-79C407B93EFE}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>12345</v>
+      </c>
+      <c r="D2">
+        <v>9999</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>12345</v>
+      </c>
+      <c r="D3">
+        <v>9999</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>